<commit_message>
Connected index page to show_plant page
</commit_message>
<xml_diff>
--- a/treebay_testing_data/plants.xlsx
+++ b/treebay_testing_data/plants.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\all\Uni\2_year_19-20\WED\Treebay\treebay_django_project\treebay_testing_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\CS\2Web\TreeBay\treebay_django_project\treebay_testing_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908787A9-635A-40E3-A8AB-9DD24B8F9CEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -167,12 +166,39 @@
   </si>
   <si>
     <t>houseplants, allergy friendly, edible</t>
+  </si>
+  <si>
+    <t>elizabeth</t>
+  </si>
+  <si>
+    <t>Ficus</t>
+  </si>
+  <si>
+    <t>Grows quite slowly. Avoid moving it around the house, unless you want to upset it.</t>
+  </si>
+  <si>
+    <t>Byres Road, Glasgow</t>
+  </si>
+  <si>
+    <t>houseplants</t>
+  </si>
+  <si>
+    <t>Mini red rose pot</t>
+  </si>
+  <si>
+    <t>Purple halanchoe</t>
+  </si>
+  <si>
+    <t>The little roses need a lot of sun.</t>
+  </si>
+  <si>
+    <t>It has been alive for 3 months without water now.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,7 +224,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,18 +247,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -248,7 +288,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -323,23 +363,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -375,23 +398,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,16 +573,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="69.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -599,7 +610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -622,7 +633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -645,7 +656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -668,7 +679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -691,7 +702,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -714,7 +725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -737,7 +748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -760,7 +771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -783,7 +794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -806,7 +817,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -829,7 +840,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -846,13 +857,83 @@
         <v>48</v>
       </c>
       <c r="F12">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Population script with images
</commit_message>
<xml_diff>
--- a/treebay_testing_data/plants.xlsx
+++ b/treebay_testing_data/plants.xlsx
@@ -186,13 +186,13 @@
     <t>Mini red rose pot</t>
   </si>
   <si>
-    <t>Purple halanchoe</t>
-  </si>
-  <si>
     <t>The little roses need a lot of sun.</t>
   </si>
   <si>
     <t>It has been alive for 3 months without water now.</t>
+  </si>
+  <si>
+    <t>Purple kalanchoe</t>
   </si>
 </sst>
 </file>
@@ -577,11 +577,12 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
     <col min="3" max="3" width="69.5546875" customWidth="1"/>
     <col min="4" max="4" width="37.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.77734375" customWidth="1"/>
@@ -894,7 +895,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
         <v>52</v>
@@ -914,10 +915,10 @@
         <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Population script with views
</commit_message>
<xml_diff>
--- a/treebay_testing_data/plants.xlsx
+++ b/treebay_testing_data/plants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>image_name</t>
-  </si>
-  <si>
     <t>Spiky boi</t>
   </si>
   <si>
@@ -105,21 +102,9 @@
     <t>Maryhill Road, Glasgow</t>
   </si>
   <si>
-    <t>Great Western Road, Glasgow</t>
-  </si>
-  <si>
     <t>Vincent Street, Glasgow</t>
   </si>
   <si>
-    <t>Buchanan Street, Glasgow</t>
-  </si>
-  <si>
-    <t>Shuna Street, Glasgow</t>
-  </si>
-  <si>
-    <t>a.png</t>
-  </si>
-  <si>
     <t>alice</t>
   </si>
   <si>
@@ -193,6 +178,18 @@
   </si>
   <si>
     <t>Purple kalanchoe</t>
+  </si>
+  <si>
+    <t>views</t>
+  </si>
+  <si>
+    <t>Gr Western Rd, Glasgow</t>
+  </si>
+  <si>
+    <t>Buchanan St, Glasgow</t>
+  </si>
+  <si>
+    <t>Shuna St, Glasgow</t>
   </si>
 </sst>
 </file>
@@ -577,7 +574,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,7 +587,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -608,329 +605,329 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>32</v>
+      <c r="G2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
-        <v>32</v>
+      <c r="G3">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>32</v>
+      <c r="G4">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F5">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
-        <v>32</v>
+      <c r="G5">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6">
         <v>15</v>
       </c>
-      <c r="G6" t="s">
-        <v>32</v>
+      <c r="G6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F7">
         <v>10</v>
       </c>
-      <c r="G7" t="s">
-        <v>32</v>
+      <c r="G7">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
-        <v>32</v>
+      <c r="G8">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
-      <c r="G9" t="s">
-        <v>32</v>
+      <c r="G9">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F10">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
-        <v>32</v>
+      <c r="G10">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F11">
         <v>6</v>
       </c>
-      <c r="G11" t="s">
-        <v>32</v>
+      <c r="G11">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F12">
         <v>9</v>
       </c>
-      <c r="G12" t="s">
-        <v>32</v>
+      <c r="G12">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
-        <v>32</v>
+      <c r="G13">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F14">
         <v>8</v>
       </c>
-      <c r="G14" t="s">
-        <v>32</v>
+      <c r="G14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
-      <c r="G15" t="s">
-        <v>32</v>
+      <c r="G15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>